<commit_message>
check in all kafs
</commit_message>
<xml_diff>
--- a/x-media/KAF1_Investitions_und_Betriebskosten.xlsx
+++ b/x-media/KAF1_Investitions_und_Betriebskosten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazyloop\Documents\GitHub\siw-bwl\x-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D891A827-47F4-4216-8C9C-C8AADCF0058E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFCED24-F082-4984-8BE9-9104465A56F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18315" yWindow="2715" windowWidth="19275" windowHeight="13305" xr2:uid="{CC08A2E5-634E-4B85-8638-C027F396722D}"/>
+    <workbookView xWindow="32820" yWindow="4530" windowWidth="28185" windowHeight="15240" xr2:uid="{CC08A2E5-634E-4B85-8638-C027F396722D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,45 +35,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
-  <si>
-    <t>Kosten Softwareentwickler</t>
-  </si>
-  <si>
-    <t>Kosten Aufbau Dev &amp; Test Umgebung</t>
-  </si>
-  <si>
-    <t>Kosten Marketingkampagne</t>
-  </si>
-  <si>
-    <t>Total Entwicklungsphase</t>
-  </si>
-  <si>
-    <t>Entwicklungsphase (14 Monate)</t>
-  </si>
-  <si>
-    <t>Markteinführung (24 Monate)</t>
-  </si>
-  <si>
-    <t>Kosten PaaS Plattform</t>
-  </si>
-  <si>
-    <t>Total Markteinführung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHF 112'800 / 2 * 2 = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHF 112'800 / 12 * 14 = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHF 800 * 24 = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHF 3'000 * 24 = </t>
-  </si>
-  <si>
-    <t>Total der Investitionskosten</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Investitionskosten</t>
+  </si>
+  <si>
+    <t>Entwicklungsaufwand = 1 FTE à 14 Monate = CHF 112'800 / 12 * 14</t>
+  </si>
+  <si>
+    <t>Total Investitionskosten</t>
+  </si>
+  <si>
+    <t>Aufbau Entwicklungs- &amp; Testumgebung</t>
+  </si>
+  <si>
+    <t>Initial-Marketing</t>
+  </si>
+  <si>
+    <t>Betriebskosten</t>
+  </si>
+  <si>
+    <t>F2 Materialkosten</t>
+  </si>
+  <si>
+    <t>F3 Raumkosten</t>
+  </si>
+  <si>
+    <t>F5 Dienstleistungskosten = Werbung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F6 kalkulatorische Kosten = CHF 700'000 / 3 Jahre = </t>
+  </si>
+  <si>
+    <t>F7 Betriebskosten pro Jahr</t>
+  </si>
+  <si>
+    <t>F4 Kapitalkosten = 5% Zins auf CHF 700'000</t>
+  </si>
+  <si>
+    <t>F5 Dienstleistungskosten = CHF 800 * 12 Monate</t>
+  </si>
+  <si>
+    <t>F1 Personalkosten = 1 * 0.5 FTE = CHF 112'800 * 0.5</t>
   </si>
 </sst>
 </file>
@@ -83,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +98,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,11 +131,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,116 +453,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8B19EF-0B80-4E64-94D8-36E2EED10B4B}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
+      <c r="A1" s="6" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>131600</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
         <v>35000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
         <v>50000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
-        <f>SUM(C2:C4)</f>
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <f>SUM(B2:B4)</f>
         <v>216600</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5">
+        <v>56400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1">
-        <v>112800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B13" s="5">
+        <v>36000</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="5">
+        <v>233333.33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1">
-        <v>19200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1">
-        <v>72000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1">
-        <f>SUM(C8:C10)</f>
-        <v>204000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3">
-        <f>SUM(C5+C11)</f>
-        <v>420600</v>
-      </c>
+      <c r="B15" s="3">
+        <f>SUM(B8:B14)</f>
+        <v>370333.32999999996</v>
+      </c>
+      <c r="C15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>